<commit_message>
made simple menu for interface
</commit_message>
<xml_diff>
--- a/testy_parsing.xlsx
+++ b/testy_parsing.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,7 +454,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="23" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="32" customWidth="1" min="2" max="2"/>
     <col width="61" customWidth="1" min="3" max="3"/>
     <col width="22" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -550,7 +550,7 @@
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t>ZUZANNA.KOWALSKA@firma.com;;jakis.email@gmail.com</t>
+          <t>ZUZANNA.KOWALSKA@firma.com||jakis.email@gmail.com</t>
         </is>
       </c>
       <c r="D3" s="4" t="n">
@@ -586,19 +586,19 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>209</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>609</v>
+        <v>304</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>409</v>
+        <v>204</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1227</v>
+        <v>612</v>
       </c>
     </row>
     <row r="5">
@@ -609,28 +609,28 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>NOWAK</t>
+          <t>ZOJA nieznane_nazwisko</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>ZOFIA.NOWAK@firma.com;jakis.email@gmail.com</t>
+          <t>ZOJA.ADAMCZYK@firma.com</t>
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>321</v>
+        <v>105</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>921</v>
+        <v>305</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>621</v>
+        <v>205</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>1863</v>
+        <v>615</v>
       </c>
     </row>
     <row r="6">
@@ -641,28 +641,28 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>PIOTROWSKA</t>
+          <t>NOWAK</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>WIKTORIA.PIOTROWSKA@firma.com</t>
+          <t>ZOFIA.NOWAK@firma.com|jakis.email@gmail.com</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>930</v>
+        <v>921</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>1890</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="7">
@@ -673,28 +673,28 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>LEWANDOWSKA</t>
+          <t>PIOTROWSKA</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>WERONIKA.LEWANDOWSKA@firma.com</t>
+          <t>WIKTORIA.PIOTROWSKA@firma.com</t>
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>625</v>
+        <v>930</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>425</v>
+        <v>630</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>1275</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="8">
@@ -705,28 +705,28 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>PAWŁOWSKA</t>
+          <t>LEWANDOWSKA</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>WANDA.PAWŁOWSKA@firma.com</t>
+          <t>WERONIKA.LEWANDOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>1287</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="9">
@@ -737,28 +737,28 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>KOWALCZYK</t>
+          <t>PAWŁOWSKA</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>URSZULA.KOWALCZYK@firma.com</t>
+          <t>WANDA.PAWŁOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D9" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>1299</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="10">
@@ -769,28 +769,28 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>SZYMAŃSKA</t>
+          <t>KOWALCZYK</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>STEFANIA.SZYMAŃSKA@firma.com</t>
+          <t>URSZULA.KOWALCZYK@firma.com</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>1311</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="11">
@@ -801,28 +801,28 @@
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>KRAWCZYK</t>
+          <t>SZYMAŃSKA</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>SOFIIA.KRAWCZYK@firma.com</t>
+          <t>STEFANIA.SZYMAŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D11" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>1323</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="12">
@@ -833,28 +833,28 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>NOWAK</t>
+          <t>KRAWCZYK</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>SOFIA.NOWAK@firma.com</t>
+          <t>SOFIIA.KRAWCZYK@firma.com</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>1335</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="13">
@@ -865,28 +865,28 @@
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>ZIELIŃSKA</t>
+          <t>NOWAK</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>SARA.ZIELIŃSKA@firma.com</t>
+          <t>SOFIA.NOWAK@firma.com</t>
         </is>
       </c>
       <c r="D13" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>1347</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="14">
@@ -897,28 +897,28 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>NOWAK</t>
+          <t>ZIELIŃSKA</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>RÓŻA.NOWAK@firma.com</t>
+          <t>SARA.ZIELIŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>1359</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="15">
@@ -929,28 +929,28 @@
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>WIŚNIEWSKA</t>
+          <t>NOWAK</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>ROZALIA.WIŚNIEWSKA@firma.com</t>
+          <t>RÓŻA.NOWAK@firma.com</t>
         </is>
       </c>
       <c r="D15" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>1371</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="16">
@@ -961,28 +961,28 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>GRABOWSKA</t>
+          <t>WIŚNIEWSKA</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>RITA.GRABOWSKA@firma.com</t>
+          <t>ROZALIA.WIŚNIEWSKA@firma.com</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="H16" s="3" t="n">
-        <v>1383</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="17">
@@ -993,28 +993,28 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>ZIELIŃSKA</t>
+          <t>GRABOWSKA</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
         <is>
-          <t>POLA.ZIELIŃSKA@firma.com</t>
+          <t>RITA.GRABOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>399</v>
+        <v>261</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>999</v>
+        <v>661</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>699</v>
+        <v>461</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>2097</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="18">
@@ -1025,28 +1025,28 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>DĄBROWSKA</t>
+          <t>ZIELIŃSKA</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>PAULINA.DĄBROWSKA@firma.com</t>
+          <t>POLA.ZIELIŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>271</v>
+        <v>399</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>671</v>
+        <v>999</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>471</v>
+        <v>699</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>1413</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="19">
@@ -1057,28 +1057,28 @@
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>LEWANDOWSKA</t>
+          <t>DĄBROWSKA</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>OLIWIA.LEWANDOWSKA@firma.com</t>
+          <t>PAULINA.DĄBROWSKA@firma.com</t>
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>414</v>
+        <v>271</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>1014</v>
+        <v>671</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>714</v>
+        <v>471</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>2142</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="20">
@@ -1089,28 +1089,28 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>KWIATKOWSKA</t>
+          <t>LEWANDOWSKA</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>OLIVIA.KWIATKOWSKA@firma.com</t>
+          <t>OLIWIA.LEWANDOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>140</v>
+        <v>414</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>681</v>
+        <v>1014</v>
       </c>
       <c r="G20" s="3" t="n">
-        <v>481</v>
+        <v>714</v>
       </c>
       <c r="H20" s="3" t="n">
-        <v>1302</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="21">
@@ -1121,28 +1121,28 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>KOWALCZYK</t>
+          <t>KWIATKOWSKA</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>NINA.KOWALCZYK@firma.com</t>
+          <t>OLIVIA.KWIATKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D21" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="G21" s="5" t="n">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>1170</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="22">
@@ -1153,12 +1153,12 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>SZYMAŃSKA</t>
+          <t>KOWALCZYK</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>NIKOLA.SZYMAŃSKA@firma.com</t>
+          <t>NINA.KOWALCZYK@firma.com</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
@@ -1168,13 +1168,13 @@
         <v>0</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="G22" s="3" t="n">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="H22" s="3" t="n">
-        <v>1178</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="23">
@@ -1185,28 +1185,28 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>ZAJĄC</t>
+          <t>SZYMAŃSKA</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>NELA.ZAJĄC@firma.com</t>
+          <t>NIKOLA.SZYMAŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>1041</v>
+        <v>689</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>741</v>
+        <v>489</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>1782</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="24">
@@ -1217,28 +1217,28 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>KAMIŃSKA</t>
+          <t>ZAJĄC</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>NEL.KAMIŃSKA@firma.com</t>
+          <t>NELA.ZAJĄC@firma.com</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E24" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>699</v>
+        <v>1041</v>
       </c>
       <c r="G24" s="3" t="n">
-        <v>499</v>
+        <v>741</v>
       </c>
       <c r="H24" s="3" t="n">
-        <v>1198</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="25">
@@ -1249,28 +1249,28 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>OLSZEWSKA</t>
+          <t>KAMIŃSKA</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>NATALIA.OLSZEWSKA@firma.com</t>
+          <t>NEL.KAMIŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>1056</v>
+        <v>699</v>
       </c>
       <c r="G25" s="5" t="n">
-        <v>756</v>
+        <v>499</v>
       </c>
       <c r="H25" s="5" t="n">
-        <v>1812</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="26">
@@ -1281,12 +1281,12 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>MAJEWSKA</t>
+          <t>OLSZEWSKA</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>NADIA.MAJEWSKA@firma.com</t>
+          <t>NATALIA.OLSZEWSKA@firma.com</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
@@ -1296,13 +1296,13 @@
         <v>0</v>
       </c>
       <c r="F26" s="3" t="n">
-        <v>1065</v>
+        <v>1056</v>
       </c>
       <c r="G26" s="3" t="n">
-        <v>765</v>
+        <v>756</v>
       </c>
       <c r="H26" s="3" t="n">
-        <v>1830</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="27">
@@ -1313,12 +1313,12 @@
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>STĘPIEŃ</t>
+          <t>MAJEWSKA</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>MILENA.STĘPIEŃ@firma.com</t>
+          <t>NADIA.MAJEWSKA@firma.com</t>
         </is>
       </c>
       <c r="D27" s="4" t="n">
@@ -1328,13 +1328,13 @@
         <v>0</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>1074</v>
+        <v>1065</v>
       </c>
       <c r="G27" s="5" t="n">
-        <v>774</v>
+        <v>765</v>
       </c>
       <c r="H27" s="5" t="n">
-        <v>1848</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="28">
@@ -1345,28 +1345,28 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>ZIELIŃSKA</t>
+          <t>STĘPIEŃ</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>MILANA.ZIELIŃSKA@firma.com</t>
+          <t>MILENA.STĘPIEŃ@firma.com</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="n">
-        <v>721</v>
+        <v>1074</v>
       </c>
       <c r="G28" s="3" t="n">
-        <v>521</v>
+        <v>774</v>
       </c>
       <c r="H28" s="3" t="n">
-        <v>1242</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="29">
@@ -1377,28 +1377,28 @@
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>WOJCIECHOWSKA</t>
+          <t>ZIELIŃSKA</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>MICHALINA.WOJCIECHOWSKA@firma.com</t>
+          <t>MILANA.ZIELIŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>1089</v>
+        <v>721</v>
       </c>
       <c r="G29" s="5" t="n">
-        <v>789</v>
+        <v>521</v>
       </c>
       <c r="H29" s="5" t="n">
-        <v>1878</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="30">
@@ -1409,12 +1409,12 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>MALINOWSKA</t>
+          <t>WOJCIECHOWSKA</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>MIA.MALINOWSKA@firma.com</t>
+          <t>MICHALINA.WOJCIECHOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
@@ -1424,13 +1424,13 @@
         <v>0</v>
       </c>
       <c r="F30" s="3" t="n">
-        <v>1098</v>
+        <v>1089</v>
       </c>
       <c r="G30" s="3" t="n">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="H30" s="3" t="n">
-        <v>1896</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="31">
@@ -1441,28 +1441,28 @@
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>ZAJĄC</t>
+          <t>MALINOWSKA</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>MELANIA.ZAJĄC@firma.com</t>
+          <t>MIA.MALINOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="5" t="n">
-        <v>737</v>
+        <v>1098</v>
       </c>
       <c r="G31" s="5" t="n">
-        <v>537</v>
+        <v>798</v>
       </c>
       <c r="H31" s="5" t="n">
-        <v>1274</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="32">
@@ -1473,12 +1473,12 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>KOZŁOWSKA</t>
+          <t>ZAJĄC</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>MATYLDA.KOZŁOWSKA@firma.com</t>
+          <t>MELANIA.ZAJĄC@firma.com</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
@@ -1488,13 +1488,13 @@
         <v>0</v>
       </c>
       <c r="F32" s="3" t="n">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="G32" s="3" t="n">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="H32" s="3" t="n">
-        <v>1282</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="33">
@@ -1505,12 +1505,12 @@
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>KWIATKOWSKA</t>
+          <t>KOZŁOWSKA</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
         <is>
-          <t>MARTYNA.KWIATKOWSKA@firma.com</t>
+          <t>MATYLDA.KOZŁOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D33" s="4" t="n">
@@ -1520,13 +1520,13 @@
         <v>0</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="G33" s="5" t="n">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>1290</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="34">
@@ -1537,28 +1537,28 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>WÓJCIK</t>
+          <t>KWIATKOWSKA</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>MARTA.WÓJCIK@firma.com</t>
+          <t>MARTYNA.KWIATKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="F34" s="3" t="n">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="G34" s="3" t="n">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="H34" s="3" t="n">
-        <v>1473</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="35">
@@ -1569,28 +1569,28 @@
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>MICHALSKA</t>
+          <t>WÓJCIK</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
         <is>
-          <t>MARIANNA.MICHALSKA@firma.com</t>
+          <t>MARTA.WÓJCIK@firma.com</t>
         </is>
       </c>
       <c r="D35" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>353</v>
+        <v>175</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="G35" s="5" t="n">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="H35" s="5" t="n">
-        <v>1659</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="36">
@@ -1601,28 +1601,28 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>DĄBROWSKA</t>
+          <t>MICHALSKA</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>MARIA.DĄBROWSKA@firma.com</t>
+          <t>MARIANNA.MICHALSKA@firma.com</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E36" s="3" t="n">
-        <v>537</v>
+        <v>353</v>
       </c>
       <c r="F36" s="3" t="n">
-        <v>1137</v>
+        <v>753</v>
       </c>
       <c r="G36" s="3" t="n">
-        <v>837</v>
+        <v>553</v>
       </c>
       <c r="H36" s="3" t="n">
-        <v>2511</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="37">
@@ -1633,28 +1633,28 @@
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>PAWŁOWSKA</t>
+          <t>DĄBROWSKA</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
         <is>
-          <t>MARCELINA.PAWŁOWSKA@firma.com</t>
+          <t>MARIA.DĄBROWSKA@firma.com</t>
         </is>
       </c>
       <c r="D37" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="F37" s="5" t="n">
-        <v>1146</v>
+        <v>1137</v>
       </c>
       <c r="G37" s="5" t="n">
-        <v>846</v>
+        <v>837</v>
       </c>
       <c r="H37" s="5" t="n">
-        <v>2538</v>
+        <v>2511</v>
       </c>
     </row>
     <row r="38">
@@ -1665,28 +1665,28 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>JAWORSKA</t>
+          <t>PAWŁOWSKA</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>MAŁGORZATA.JAWORSKA@firma.com</t>
+          <t>MARCELINA.PAWŁOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="3" t="n">
-        <v>369</v>
+        <v>546</v>
       </c>
       <c r="F38" s="3" t="n">
-        <v>769</v>
+        <v>1146</v>
       </c>
       <c r="G38" s="3" t="n">
-        <v>569</v>
+        <v>846</v>
       </c>
       <c r="H38" s="3" t="n">
-        <v>1707</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="39">
@@ -1697,28 +1697,28 @@
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>LEWANDOWSKA</t>
+          <t>JAWORSKA</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
         <is>
-          <t>MALWINA.LEWANDOWSKA@firma.com</t>
+          <t>MAŁGORZATA.JAWORSKA@firma.com</t>
         </is>
       </c>
       <c r="D39" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F39" s="5" t="n">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="G39" s="5" t="n">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="H39" s="5" t="n">
-        <v>1719</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="40">
@@ -1729,28 +1729,28 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>KOWALCZYK</t>
+          <t>LEWANDOWSKA</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>MAJA.KOWALCZYK@firma.com</t>
+          <t>MALWINA.LEWANDOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E40" s="3" t="n">
-        <v>567</v>
+        <v>373</v>
       </c>
       <c r="F40" s="3" t="n">
-        <v>1167</v>
+        <v>773</v>
       </c>
       <c r="G40" s="3" t="n">
-        <v>867</v>
+        <v>573</v>
       </c>
       <c r="H40" s="3" t="n">
-        <v>2601</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="41">
@@ -1761,28 +1761,28 @@
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>KRÓL</t>
+          <t>KOWALCZYK</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
         <is>
-          <t>MAGDALENA.KRÓL@firma.com</t>
+          <t>MAJA.KOWALCZYK@firma.com</t>
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>383</v>
+        <v>567</v>
       </c>
       <c r="F41" s="5" t="n">
-        <v>783</v>
+        <v>1167</v>
       </c>
       <c r="G41" s="5" t="n">
-        <v>583</v>
+        <v>867</v>
       </c>
       <c r="H41" s="5" t="n">
-        <v>1749</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="42">
@@ -1793,28 +1793,28 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>JABŁOŃSKA</t>
+          <t>KRÓL</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>ŁUCJA.JABŁOŃSKA@firma.com</t>
+          <t>MAGDALENA.KRÓL@firma.com</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42" s="3" t="n">
-        <v>582</v>
+        <v>383</v>
       </c>
       <c r="F42" s="3" t="n">
-        <v>393</v>
+        <v>783</v>
       </c>
       <c r="G42" s="3" t="n">
-        <v>882</v>
+        <v>583</v>
       </c>
       <c r="H42" s="3" t="n">
-        <v>1857</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="43">
@@ -1825,28 +1825,28 @@
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>PIOTROWSKA</t>
+          <t>JABŁOŃSKA</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
         <is>
-          <t>LUIZA.PIOTROWSKA@firma.com</t>
+          <t>ŁUCJA.JABŁOŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="5" t="n">
+        <v>582</v>
+      </c>
+      <c r="F43" s="5" t="n">
         <v>393</v>
       </c>
-      <c r="F43" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="G43" s="5" t="n">
-        <v>593</v>
+        <v>882</v>
       </c>
       <c r="H43" s="5" t="n">
-        <v>986</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="44">
@@ -1857,28 +1857,28 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>MAZUR</t>
+          <t>PIOTROWSKA</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>LIWIA.MAZUR@firma.com</t>
+          <t>LUIZA.PIOTROWSKA@firma.com</t>
         </is>
       </c>
       <c r="D44" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E44" s="3" t="n">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F44" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G44" s="3" t="n">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="H44" s="3" t="n">
-        <v>994</v>
+        <v>986</v>
       </c>
     </row>
     <row r="45">
@@ -1889,28 +1889,28 @@
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>JAWORSKA</t>
+          <t>MAZUR</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
         <is>
-          <t>LILIANNA.JAWORSKA@firma.com</t>
+          <t>LIWIA.MAZUR@firma.com</t>
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>603</v>
+        <v>397</v>
       </c>
       <c r="F45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G45" s="5" t="n">
-        <v>903</v>
+        <v>597</v>
       </c>
       <c r="H45" s="5" t="n">
-        <v>1506</v>
+        <v>994</v>
       </c>
     </row>
     <row r="46">
@@ -1921,28 +1921,28 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>KACZMAREK</t>
+          <t>JAWORSKA</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>LILIANA.KACZMAREK@firma.com</t>
+          <t>LILIANNA.JAWORSKA@firma.com</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E46" s="3" t="n">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="F46" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G46" s="3" t="n">
-        <v>912</v>
+        <v>903</v>
       </c>
       <c r="H46" s="3" t="n">
-        <v>1524</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="47">
@@ -1953,28 +1953,28 @@
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>JANKOWSKA</t>
+          <t>KACZMAREK</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
         <is>
-          <t>LILIA.JANKOWSKA@firma.com</t>
+          <t>LILIANA.KACZMAREK@firma.com</t>
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>413</v>
+        <v>612</v>
       </c>
       <c r="F47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G47" s="5" t="n">
-        <v>613</v>
+        <v>912</v>
       </c>
       <c r="H47" s="5" t="n">
-        <v>1026</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="48">
@@ -1985,28 +1985,28 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>STĘPIEŃ</t>
+          <t>JANKOWSKA</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>LIDIA.STĘPIEŃ@firma.com</t>
+          <t>LILIA.JANKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D48" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E48" s="3" t="n">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F48" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G48" s="3" t="n">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H48" s="3" t="n">
-        <v>1034</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="49">
@@ -2017,28 +2017,28 @@
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>WOŹNIAK</t>
+          <t>STĘPIEŃ</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>LENA.WOŹNIAK@firma.com</t>
+          <t>LIDIA.STĘPIEŃ@firma.com</t>
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>633</v>
+        <v>417</v>
       </c>
       <c r="F49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G49" s="5" t="n">
-        <v>933</v>
+        <v>617</v>
       </c>
       <c r="H49" s="5" t="n">
-        <v>1566</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="50">
@@ -2049,28 +2049,28 @@
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>ZAJĄC</t>
+          <t>WOŹNIAK</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>LEA.ZAJĄC@firma.com</t>
+          <t>LENA.WOŹNIAK@firma.com</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E50" s="3" t="n">
-        <v>427</v>
+        <v>633</v>
       </c>
       <c r="F50" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G50" s="3" t="n">
-        <v>627</v>
+        <v>933</v>
       </c>
       <c r="H50" s="3" t="n">
-        <v>1054</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="51">
@@ -2081,28 +2081,28 @@
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>WIŚNIEWSKA</t>
+          <t>ZAJĄC</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
         <is>
-          <t>LAURA.WIŚNIEWSKA@firma.com;;jakis.email@gmail.com</t>
+          <t>LEA.ZAJĄC@firma.com</t>
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>648</v>
+        <v>427</v>
       </c>
       <c r="F51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="5" t="n">
-        <v>948</v>
+        <v>627</v>
       </c>
       <c r="H51" s="5" t="n">
-        <v>1596</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="52">
@@ -2113,28 +2113,28 @@
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>KRÓL</t>
+          <t>WIŚNIEWSKA</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>LARA.KRÓL@firma.com</t>
+          <t>LAURA.WIŚNIEWSKA@firma.com||jakis.email@gmail.com</t>
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>437</v>
+        <v>648</v>
       </c>
       <c r="F52" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="3" t="n">
-        <v>637</v>
+        <v>948</v>
       </c>
       <c r="H52" s="3" t="n">
-        <v>1074</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="53">
@@ -2145,28 +2145,28 @@
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>WIECZOREK</t>
+          <t>KRÓL</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
         <is>
-          <t>KORNELIA.WIECZOREK@firma.com</t>
+          <t>LARA.KRÓL@firma.com</t>
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>663</v>
+        <v>437</v>
       </c>
       <c r="F53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="5" t="n">
-        <v>963</v>
+        <v>637</v>
       </c>
       <c r="H53" s="5" t="n">
-        <v>1626</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="54">
@@ -2177,28 +2177,28 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>KACZMAREK</t>
+          <t>WIECZOREK</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>KLAUDIA.KACZMAREK@firma.com</t>
+          <t>KORNELIA.WIECZOREK@firma.com</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>447</v>
+        <v>663</v>
       </c>
       <c r="F54" s="3" t="n">
-        <v>424</v>
+        <v>0</v>
       </c>
       <c r="G54" s="3" t="n">
-        <v>647</v>
+        <v>963</v>
       </c>
       <c r="H54" s="3" t="n">
-        <v>1518</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="55">
@@ -2209,28 +2209,28 @@
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>KWIATKOWSKA</t>
+          <t>KACZMAREK</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
         <is>
-          <t>KLARA.KWIATKOWSKA@firma.com</t>
+          <t>KLAUDIA.KACZMAREK@firma.com</t>
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>678</v>
+        <v>447</v>
       </c>
       <c r="F55" s="5" t="n">
-        <v>1278</v>
+        <v>424</v>
       </c>
       <c r="G55" s="5" t="n">
-        <v>978</v>
+        <v>647</v>
       </c>
       <c r="H55" s="5" t="n">
-        <v>2934</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="56">
@@ -2241,28 +2241,28 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>WIECZOREK</t>
+          <t>KWIATKOWSKA</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>KINGA.WIECZOREK@firma.com</t>
+          <t>KLARA.KWIATKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" s="3" t="n">
-        <v>457</v>
+        <v>678</v>
       </c>
       <c r="F56" s="3" t="n">
-        <v>857</v>
+        <v>1278</v>
       </c>
       <c r="G56" s="3" t="n">
-        <v>657</v>
+        <v>978</v>
       </c>
       <c r="H56" s="3" t="n">
-        <v>1971</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="57">
@@ -2273,28 +2273,28 @@
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>WOŹNIAK</t>
+          <t>WIECZOREK</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
         <is>
-          <t>KATARZYNA.WOŹNIAK@firma.com</t>
+          <t>KINGA.WIECZOREK@firma.com</t>
         </is>
       </c>
       <c r="D57" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="F57" s="5" t="n">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="G57" s="5" t="n">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="H57" s="5" t="n">
-        <v>1983</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="58">
@@ -2305,28 +2305,28 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>JANKOWSKA</t>
+          <t>WOŹNIAK</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>KAROLINA.JANKOWSKA@firma.com</t>
+          <t>KATARZYNA.WOŹNIAK@firma.com</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E58" s="3" t="n">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F58" s="3" t="n">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="G58" s="3" t="n">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="H58" s="3" t="n">
-        <v>1995</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="59">
@@ -2337,28 +2337,28 @@
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>MICHALSKA</t>
+          <t>JANKOWSKA</t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
         <is>
-          <t>KAMILA.MICHALSKA@firma.com</t>
+          <t>KAROLINA.JANKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D59" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F59" s="5" t="n">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="G59" s="5" t="n">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="H59" s="5" t="n">
-        <v>2007</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="60">
@@ -2369,28 +2369,28 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>NOWAKOWSKA</t>
+          <t>MICHALSKA</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>KALINA.NOWAKOWSKA@firma.com</t>
+          <t>KAMILA.MICHALSKA@firma.com</t>
         </is>
       </c>
       <c r="D60" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F60" s="3" t="n">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="G60" s="3" t="n">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="H60" s="3" t="n">
-        <v>2019</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="61">
@@ -2401,28 +2401,28 @@
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>KOWALSKA</t>
+          <t>NOWAKOWSKA</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
         <is>
-          <t>KAJA.KOWALSKA@firma.com</t>
+          <t>KALINA.NOWAKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D61" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F61" s="5" t="n">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="G61" s="5" t="n">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="H61" s="5" t="n">
-        <v>2031</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="62">
@@ -2433,28 +2433,28 @@
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>KAMIŃSKA</t>
+          <t>KOWALSKA</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>JULIA.KAMIŃSKA@firma.com</t>
+          <t>KAJA.KOWALSKA@firma.com</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" s="3" t="n">
-        <v>723</v>
+        <v>477</v>
       </c>
       <c r="F62" s="3" t="n">
-        <v>1323</v>
+        <v>877</v>
       </c>
       <c r="G62" s="3" t="n">
-        <v>1023</v>
+        <v>677</v>
       </c>
       <c r="H62" s="3" t="n">
-        <v>3069</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="63">
@@ -2465,28 +2465,28 @@
       </c>
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>MAJEWSKA</t>
+          <t>KAMIŃSKA</t>
         </is>
       </c>
       <c r="C63" s="4" t="inlineStr">
         <is>
-          <t>JOANNA.MAJEWSKA@firma.com</t>
+          <t>JULIA.KAMIŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>487</v>
+        <v>723</v>
       </c>
       <c r="F63" s="5" t="n">
-        <v>887</v>
+        <v>1323</v>
       </c>
       <c r="G63" s="5" t="n">
-        <v>687</v>
+        <v>1023</v>
       </c>
       <c r="H63" s="5" t="n">
-        <v>2061</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="64">
@@ -2497,28 +2497,28 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>PIOTROWSKA</t>
+          <t>MAJEWSKA</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>JAŚMINA.PIOTROWSKA@firma.com</t>
+          <t>JOANNA.MAJEWSKA@firma.com</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E64" s="3" t="n">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F64" s="3" t="n">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="G64" s="3" t="n">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="H64" s="3" t="n">
-        <v>2073</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="65">
@@ -2529,28 +2529,28 @@
       </c>
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>ADAMCZYK</t>
+          <t>PIOTROWSKA</t>
         </is>
       </c>
       <c r="C65" s="4" t="inlineStr">
         <is>
-          <t>JAGODA.ADAMCZYK@firma.com</t>
+          <t>JAŚMINA.PIOTROWSKA@firma.com</t>
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>744</v>
+        <v>491</v>
       </c>
       <c r="F65" s="5" t="n">
-        <v>1344</v>
+        <v>891</v>
       </c>
       <c r="G65" s="5" t="n">
-        <v>1044</v>
+        <v>691</v>
       </c>
       <c r="H65" s="5" t="n">
-        <v>3132</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="66">
@@ -2561,28 +2561,28 @@
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>PAWŁOWSKA</t>
+          <t>ADAMCZYK</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>JAGNA.PAWŁOWSKA@firma.com</t>
+          <t>JAGODA.ADAMCZYK@firma.com</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>501</v>
+        <v>744</v>
       </c>
       <c r="F66" s="3" t="n">
-        <v>901</v>
+        <v>1344</v>
       </c>
       <c r="G66" s="3" t="n">
-        <v>701</v>
+        <v>1044</v>
       </c>
       <c r="H66" s="3" t="n">
-        <v>2103</v>
+        <v>3132</v>
       </c>
     </row>
     <row r="67">
@@ -2593,28 +2593,28 @@
       </c>
       <c r="B67" s="4" t="inlineStr">
         <is>
-          <t>WRÓBEL</t>
+          <t>PAWŁOWSKA</t>
         </is>
       </c>
       <c r="C67" s="4" t="inlineStr">
         <is>
-          <t>IZABELA.WRÓBEL@firma.com</t>
+          <t>JAGNA.PAWŁOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D67" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F67" s="5" t="n">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="G67" s="5" t="n">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="H67" s="5" t="n">
-        <v>2115</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="68">
@@ -2625,28 +2625,28 @@
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>KRAWCZYK</t>
+          <t>WRÓBEL</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>IGA.KRAWCZYK@firma.com;;jakis.email@gmail.com</t>
+          <t>IZABELA.WRÓBEL@firma.com</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>765</v>
+        <v>505</v>
       </c>
       <c r="F68" s="3" t="n">
-        <v>1365</v>
+        <v>905</v>
       </c>
       <c r="G68" s="3" t="n">
-        <v>1065</v>
+        <v>705</v>
       </c>
       <c r="H68" s="3" t="n">
-        <v>3195</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="69">
@@ -2657,28 +2657,28 @@
       </c>
       <c r="B69" s="4" t="inlineStr">
         <is>
-          <t>KOZŁOWSKA</t>
+          <t>KRAWCZYK</t>
         </is>
       </c>
       <c r="C69" s="4" t="inlineStr">
         <is>
-          <t>IDA.KOZŁOWSKA@firma.com</t>
+          <t>IGA.KRAWCZYK@firma.com||jakis.email@gmail.com</t>
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>515</v>
+        <v>765</v>
       </c>
       <c r="F69" s="5" t="n">
-        <v>915</v>
+        <v>1365</v>
       </c>
       <c r="G69" s="5" t="n">
-        <v>715</v>
+        <v>1065</v>
       </c>
       <c r="H69" s="5" t="n">
-        <v>2145</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="70">
@@ -2689,28 +2689,28 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>GRABOWSKA</t>
+          <t>KOZŁOWSKA</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>HELENA.GRABOWSKA@firma.com</t>
+          <t>IDA.KOZŁOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E70" s="3" t="n">
-        <v>780</v>
+        <v>515</v>
       </c>
       <c r="F70" s="3" t="n">
-        <v>1380</v>
+        <v>915</v>
       </c>
       <c r="G70" s="3" t="n">
-        <v>1080</v>
+        <v>715</v>
       </c>
       <c r="H70" s="3" t="n">
-        <v>3240</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="71">
@@ -2721,28 +2721,28 @@
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t>WÓJCIK</t>
+          <t>GRABOWSKA</t>
         </is>
       </c>
       <c r="C71" s="4" t="inlineStr">
         <is>
-          <t>HANNA.WÓJCIK@firma.com</t>
+          <t>HELENA.GRABOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D71" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E71" s="5" t="n">
-        <v>789</v>
+        <v>780</v>
       </c>
       <c r="F71" s="5" t="n">
-        <v>1389</v>
+        <v>1380</v>
       </c>
       <c r="G71" s="5" t="n">
-        <v>1089</v>
+        <v>1080</v>
       </c>
       <c r="H71" s="5" t="n">
-        <v>3267</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="72">
@@ -2753,28 +2753,28 @@
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>GRABOWSKA</t>
+          <t>WÓJCIK</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>GAJA.GRABOWSKA@firma.com</t>
+          <t>HANNA.WÓJCIK@firma.com</t>
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E72" s="3" t="n">
-        <v>531</v>
+        <v>789</v>
       </c>
       <c r="F72" s="3" t="n">
-        <v>931</v>
+        <v>1389</v>
       </c>
       <c r="G72" s="3" t="n">
-        <v>731</v>
+        <v>1089</v>
       </c>
       <c r="H72" s="3" t="n">
-        <v>2193</v>
+        <v>3267</v>
       </c>
     </row>
     <row r="73">
@@ -2785,28 +2785,28 @@
       </c>
       <c r="B73" s="4" t="inlineStr">
         <is>
-          <t>MICHALSKA</t>
+          <t>GRABOWSKA</t>
         </is>
       </c>
       <c r="C73" s="4" t="inlineStr">
         <is>
-          <t>GABRIELA.MICHALSKA@firma.com</t>
+          <t>GAJA.GRABOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E73" s="5" t="n">
-        <v>804</v>
+        <v>531</v>
       </c>
       <c r="F73" s="5" t="n">
-        <v>1404</v>
+        <v>931</v>
       </c>
       <c r="G73" s="5" t="n">
-        <v>1104</v>
+        <v>731</v>
       </c>
       <c r="H73" s="5" t="n">
-        <v>3312</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="74">
@@ -2817,28 +2817,28 @@
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>KOWALSKA</t>
+          <t>MICHALSKA</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>EWA.KOWALSKA@firma.com</t>
+          <t>GABRIELA.MICHALSKA@firma.com</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>541</v>
+        <v>804</v>
       </c>
       <c r="F74" s="3" t="n">
-        <v>941</v>
+        <v>1404</v>
       </c>
       <c r="G74" s="3" t="n">
-        <v>741</v>
+        <v>1104</v>
       </c>
       <c r="H74" s="3" t="n">
-        <v>2223</v>
+        <v>3312</v>
       </c>
     </row>
     <row r="75">
@@ -2849,28 +2849,28 @@
       </c>
       <c r="B75" s="4" t="inlineStr">
         <is>
-          <t>WOJCIECHOWSKA</t>
+          <t>KOWALSKA</t>
         </is>
       </c>
       <c r="C75" s="4" t="inlineStr">
         <is>
-          <t>EMMA.WOJCIECHOWSKA@firma.com</t>
+          <t>EWA.KOWALSKA@firma.com</t>
         </is>
       </c>
       <c r="D75" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E75" s="5" t="n">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F75" s="5" t="n">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="G75" s="5" t="n">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="H75" s="5" t="n">
-        <v>2235</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="76">
@@ -2881,28 +2881,28 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>MAZUR</t>
+          <t>WOJCIECHOWSKA</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>EMILIA.MAZUR@firma.com</t>
+          <t>EMMA.WOJCIECHOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E76" s="3" t="n">
-        <v>825</v>
+        <v>545</v>
       </c>
       <c r="F76" s="3" t="n">
-        <v>1425</v>
+        <v>945</v>
       </c>
       <c r="G76" s="3" t="n">
-        <v>1125</v>
+        <v>745</v>
       </c>
       <c r="H76" s="3" t="n">
-        <v>3375</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="77">
@@ -2913,28 +2913,28 @@
       </c>
       <c r="B77" s="4" t="inlineStr">
         <is>
-          <t>KRAWCZYK</t>
+          <t>MAZUR</t>
         </is>
       </c>
       <c r="C77" s="4" t="inlineStr">
         <is>
-          <t>ELIZA.KRAWCZYK@firma.com</t>
+          <t>EMILIA.MAZUR@firma.com</t>
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E77" s="5" t="n">
-        <v>555</v>
+        <v>825</v>
       </c>
       <c r="F77" s="5" t="n">
-        <v>955</v>
+        <v>1425</v>
       </c>
       <c r="G77" s="5" t="n">
-        <v>755</v>
+        <v>1125</v>
       </c>
       <c r="H77" s="5" t="n">
-        <v>2265</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="78">
@@ -2945,28 +2945,28 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>WIŚNIEWSKA</t>
+          <t>KRAWCZYK</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>DOMINIKA.WIŚNIEWSKA@firma.com</t>
+          <t>ELIZA.KRAWCZYK@firma.com</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E78" s="3" t="n">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F78" s="3" t="n">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="G78" s="3" t="n">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="H78" s="3" t="n">
-        <v>2277</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="79">
@@ -2977,28 +2977,28 @@
       </c>
       <c r="B79" s="4" t="inlineStr">
         <is>
-          <t>OLSZEWSKA</t>
+          <t>WIŚNIEWSKA</t>
         </is>
       </c>
       <c r="C79" s="4" t="inlineStr">
         <is>
-          <t>DIANA.OLSZEWSKA@firma.com</t>
+          <t>DOMINIKA.WIŚNIEWSKA@firma.com</t>
         </is>
       </c>
       <c r="D79" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E79" s="5" t="n">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="F79" s="5" t="n">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="G79" s="5" t="n">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="H79" s="5" t="n">
-        <v>2289</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="80">
@@ -3009,28 +3009,28 @@
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>MAZUR</t>
+          <t>OLSZEWSKA</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>DARIA.MAZUR@firma.com</t>
+          <t>DIANA.OLSZEWSKA@firma.com</t>
         </is>
       </c>
       <c r="D80" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="F80" s="3" t="n">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="G80" s="3" t="n">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="H80" s="3" t="n">
-        <v>2301</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="81">
@@ -3041,28 +3041,28 @@
       </c>
       <c r="B81" s="4" t="inlineStr">
         <is>
-          <t>WRÓBEL</t>
+          <t>MAZUR</t>
         </is>
       </c>
       <c r="C81" s="4" t="inlineStr">
         <is>
-          <t>BLANKA.WRÓBEL@firma.com</t>
+          <t>DARIA.MAZUR@firma.com</t>
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E81" s="5" t="n">
-        <v>858</v>
+        <v>567</v>
       </c>
       <c r="F81" s="5" t="n">
-        <v>1458</v>
+        <v>967</v>
       </c>
       <c r="G81" s="5" t="n">
-        <v>1158</v>
+        <v>767</v>
       </c>
       <c r="H81" s="5" t="n">
-        <v>3474</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="82">
@@ -3073,28 +3073,28 @@
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>JABŁOŃSKA</t>
+          <t>WRÓBEL</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>BIANKA.JABŁOŃSKA@firma.com</t>
+          <t>BLANKA.WRÓBEL@firma.com</t>
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E82" s="3" t="n">
-        <v>577</v>
+        <v>858</v>
       </c>
       <c r="F82" s="3" t="n">
-        <v>977</v>
+        <v>1458</v>
       </c>
       <c r="G82" s="3" t="n">
-        <v>777</v>
+        <v>1158</v>
       </c>
       <c r="H82" s="3" t="n">
-        <v>2331</v>
+        <v>3474</v>
       </c>
     </row>
     <row r="83">
@@ -3105,28 +3105,28 @@
       </c>
       <c r="B83" s="4" t="inlineStr">
         <is>
-          <t>DĄBROWSKA</t>
+          <t>JABŁOŃSKA</t>
         </is>
       </c>
       <c r="C83" s="4" t="inlineStr">
         <is>
-          <t>BARBARA.DĄBROWSKA@firma.com</t>
+          <t>BIANKA.JABŁOŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D83" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E83" s="5" t="n">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="F83" s="5" t="n">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="G83" s="5" t="n">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="H83" s="5" t="n">
-        <v>2343</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="84">
@@ -3137,28 +3137,28 @@
       </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>WOŹNIAK</t>
+          <t>DĄBROWSKA</t>
         </is>
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>AURELIA.WOŹNIAK@firma.com</t>
+          <t>BARBARA.DĄBROWSKA@firma.com</t>
         </is>
       </c>
       <c r="D84" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="F84" s="3" t="n">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="G84" s="3" t="n">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="H84" s="3" t="n">
-        <v>2355</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="85">
@@ -3169,28 +3169,28 @@
       </c>
       <c r="B85" s="4" t="inlineStr">
         <is>
-          <t>MALINOWSKA</t>
+          <t>WOŹNIAK</t>
         </is>
       </c>
       <c r="C85" s="4" t="inlineStr">
         <is>
-          <t>APOLONIA.MALINOWSKA@firma.com</t>
+          <t>AURELIA.WOŹNIAK@firma.com</t>
         </is>
       </c>
       <c r="D85" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E85" s="5" t="n">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="F85" s="5" t="n">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="G85" s="5" t="n">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="H85" s="5" t="n">
-        <v>2367</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="86">
@@ -3201,28 +3201,28 @@
       </c>
       <c r="B86" s="2" t="inlineStr">
         <is>
-          <t>KOZŁOWSKA</t>
+          <t>MALINOWSKA</t>
         </is>
       </c>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>ANTONINA.KOZŁOWSKA@firma.com;;jakis.email@gmail.com</t>
+          <t>APOLONIA.MALINOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>891</v>
+        <v>589</v>
       </c>
       <c r="F86" s="3" t="n">
-        <v>1491</v>
+        <v>989</v>
       </c>
       <c r="G86" s="3" t="n">
-        <v>1191</v>
+        <v>789</v>
       </c>
       <c r="H86" s="3" t="n">
-        <v>3573</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="87">
@@ -3233,28 +3233,28 @@
       </c>
       <c r="B87" s="4" t="inlineStr">
         <is>
-          <t>NOWAKOWSKA</t>
+          <t>KOZŁOWSKA</t>
         </is>
       </c>
       <c r="C87" s="4" t="inlineStr">
         <is>
-          <t>ANNA.NOWAKOWSKA@firma.com</t>
+          <t>ANTONINA.KOZŁOWSKA@firma.com||jakis.email@gmail.com</t>
         </is>
       </c>
       <c r="D87" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E87" s="5" t="n">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="F87" s="5" t="n">
-        <v>1500</v>
+        <v>1491</v>
       </c>
       <c r="G87" s="5" t="n">
-        <v>1200</v>
+        <v>1191</v>
       </c>
       <c r="H87" s="5" t="n">
-        <v>3600</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="88">
@@ -3265,28 +3265,28 @@
       </c>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>KAMIŃSKA</t>
+          <t>NOWAKOWSKA</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>ANIELA.KAMIŃSKA@firma.com</t>
+          <t>ANNA.NOWAKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E88" s="3" t="n">
-        <v>605</v>
+        <v>900</v>
       </c>
       <c r="F88" s="3" t="n">
-        <v>1005</v>
+        <v>1500</v>
       </c>
       <c r="G88" s="3" t="n">
-        <v>805</v>
+        <v>1200</v>
       </c>
       <c r="H88" s="3" t="n">
-        <v>2415</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="89">
@@ -3297,28 +3297,28 @@
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>WÓJCIK</t>
+          <t>KAMIŃSKA</t>
         </is>
       </c>
       <c r="C89" s="4" t="inlineStr">
         <is>
-          <t>ANASTAZJA.WÓJCIK@firma.com</t>
+          <t>ANIELA.KAMIŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D89" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E89" s="5" t="n">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="F89" s="5" t="n">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="G89" s="5" t="n">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="H89" s="5" t="n">
-        <v>2427</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="90">
@@ -3329,28 +3329,28 @@
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>JANKOWSKA</t>
+          <t>WÓJCIK</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>AMELIA.JANKOWSKA@firma.com</t>
+          <t>ANASTAZJA.WÓJCIK@firma.com</t>
         </is>
       </c>
       <c r="D90" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="F90" s="3" t="n">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="G90" s="3" t="n">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="H90" s="3" t="n">
-        <v>2439</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="91">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="B91" s="4" t="inlineStr">
         <is>
-          <t>JANKOWSKA-Dobra</t>
+          <t>JANKOWSKA</t>
         </is>
       </c>
       <c r="C91" s="4" t="inlineStr">
@@ -3370,19 +3370,19 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E91" s="5" t="n">
-        <v>308</v>
+        <v>613</v>
       </c>
       <c r="F91" s="5" t="n">
-        <v>508</v>
+        <v>1013</v>
       </c>
       <c r="G91" s="5" t="n">
-        <v>408</v>
+        <v>813</v>
       </c>
       <c r="H91" s="5" t="n">
-        <v>1224</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="92">
@@ -3393,28 +3393,28 @@
       </c>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>SZYMAŃSKA</t>
+          <t>JANKOWSKA-Dobra</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>ALICJA.SZYMAŃSKA@firma.com</t>
+          <t>AMELIA.JANKOWSKA@firma.com</t>
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>930</v>
+        <v>308</v>
       </c>
       <c r="F92" s="3" t="n">
-        <v>1530</v>
+        <v>508</v>
       </c>
       <c r="G92" s="3" t="n">
-        <v>1230</v>
+        <v>408</v>
       </c>
       <c r="H92" s="3" t="n">
-        <v>3690</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="93">
@@ -3425,28 +3425,28 @@
       </c>
       <c r="B93" s="4" t="inlineStr">
         <is>
-          <t>KRÓL</t>
+          <t>SZYMAŃSKA</t>
         </is>
       </c>
       <c r="C93" s="4" t="inlineStr">
         <is>
-          <t>ALEKSANDRA.KRÓL@firma.com</t>
+          <t>ALICJA.SZYMAŃSKA@firma.com</t>
         </is>
       </c>
       <c r="D93" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E93" s="5" t="n">
-        <v>939</v>
+        <v>930</v>
       </c>
       <c r="F93" s="5" t="n">
-        <v>1539</v>
+        <v>1530</v>
       </c>
       <c r="G93" s="5" t="n">
-        <v>1239</v>
+        <v>1230</v>
       </c>
       <c r="H93" s="5" t="n">
-        <v>3717</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="94">
@@ -3457,28 +3457,28 @@
       </c>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>WOJCIECHOWSKA</t>
+          <t>KRÓL</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>AGATA.WOJCIECHOWSKA@firma.com</t>
+          <t>ALEKSANDRA.KRÓL@firma.com</t>
         </is>
       </c>
       <c r="D94" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E94" s="3" t="n">
-        <v>631</v>
+        <v>939</v>
       </c>
       <c r="F94" s="3" t="n">
-        <v>1031</v>
+        <v>1539</v>
       </c>
       <c r="G94" s="3" t="n">
-        <v>831</v>
+        <v>1239</v>
       </c>
       <c r="H94" s="3" t="n">
-        <v>2493</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="95">
@@ -3489,27 +3489,59 @@
       </c>
       <c r="B95" s="4" t="inlineStr">
         <is>
+          <t>WOJCIECHOWSKA</t>
+        </is>
+      </c>
+      <c r="C95" s="4" t="inlineStr">
+        <is>
+          <t>AGATA.WOJCIECHOWSKA@firma.com</t>
+        </is>
+      </c>
+      <c r="D95" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E95" s="5" t="n">
+        <v>631</v>
+      </c>
+      <c r="F95" s="5" t="n">
+        <v>1031</v>
+      </c>
+      <c r="G95" s="5" t="n">
+        <v>831</v>
+      </c>
+      <c r="H95" s="5" t="n">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>Szanowna Pani</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
           <t>KACZMAREK</t>
         </is>
       </c>
-      <c r="C95" s="4" t="inlineStr">
+      <c r="C96" s="2" t="inlineStr">
         <is>
           <t>ADRIANNA.KACZMAREK@firma.com</t>
         </is>
       </c>
-      <c r="D95" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E95" s="5" t="n">
+      <c r="D96" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E96" s="3" t="n">
         <v>635</v>
       </c>
-      <c r="F95" s="5" t="n">
+      <c r="F96" s="3" t="n">
         <v>1035</v>
       </c>
-      <c r="G95" s="5" t="n">
+      <c r="G96" s="3" t="n">
         <v>835</v>
       </c>
-      <c r="H95" s="5" t="n">
+      <c r="H96" s="3" t="n">
         <v>2505</v>
       </c>
     </row>

</xml_diff>